<commit_message>
initial apparently working version
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionBook/Scores-A4.xlsx
+++ b/owlcms/src/main/resources/templates/competitionBook/Scores-A4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC14C4EA-B830-4711-BD84-5F3D88BB4EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392468D6-4F8C-4FF4-B2EB-E0875A30CCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="447" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="447" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="35" r:id="rId1"/>
@@ -334,12 +334,6 @@
     <t>&lt;jx:forEach items="${mCustom}" var="l" varStatus="lifterLoop"&gt;</t>
   </si>
   <si>
-    <t>${l.customScoreComputed}</t>
-  </si>
-  <si>
-    <t>${l.customRank}</t>
-  </si>
-  <si>
     <t>$[if(D12="M",if(C17&lt;&gt;"",if(k12&lt;=C17,j12,0),if(k12&gt;0,j12,0)),if(C18&lt;&gt;"",if(k12&lt;=C18,j12,0),if(k12&gt;0,j12,0)))]</t>
   </si>
   <si>
@@ -529,7 +523,13 @@
     <t>${l.totalRank &lt; 0 ? t.get("Results.Extra/Invited") : l.totalRank}</t>
   </si>
   <si>
-    <t>${l.customRank &lt; 0 ? t.get("Results.Extra/Invited") : l.customRank}</t>
+    <t>${l.categoryScore}</t>
+  </si>
+  <si>
+    <t>${l.categoryScoreRank &lt; 0 ? t.get("Results.Extra/Invited") : (l.categoryScoreRank &gt; 0 ? l.categoryScoreRank : "" )}</t>
+  </si>
+  <si>
+    <t>${l.categoryScoreRank}</t>
   </si>
 </sst>
 </file>
@@ -2290,7 +2290,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="104" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="104"/>
       <c r="D3" s="104"/>
@@ -3923,7 +3923,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="86" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="91" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -3939,7 +3939,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3957,7 +3957,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3994,13 +3994,13 @@
         <v>42</v>
       </c>
       <c r="N3" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="O3" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="P3" s="64" t="s">
         <v>146</v>
-      </c>
-      <c r="O3" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="P3" s="64" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -4023,10 +4023,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" s="35" t="s">
         <v>14</v>
@@ -4042,13 +4042,13 @@
         <v>9</v>
       </c>
       <c r="N5" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="P5" s="102" t="s">
         <v>149</v>
-      </c>
-      <c r="O5" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="P5" s="102" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4116,13 +4116,13 @@
         <v>46</v>
       </c>
       <c r="H10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>50</v>
@@ -4134,18 +4134,18 @@
         <v>51</v>
       </c>
       <c r="N10" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="O10" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="P10" s="64" t="s">
         <v>146</v>
-      </c>
-      <c r="O10" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="P10" s="64" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -4180,31 +4180,31 @@
         <v>4</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>39</v>
       </c>
       <c r="L12" s="62" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M12" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N12" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="O12" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="N12" s="62" t="s">
+      <c r="P12" s="62" t="s">
         <v>153</v>
-      </c>
-      <c r="O12" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="P12" s="62" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4254,7 +4254,7 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -4324,7 +4324,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="74" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="67" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -4366,13 +4366,13 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:24" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J2" s="66"/>
     </row>
@@ -4402,28 +4402,28 @@
     </row>
     <row r="4" spans="1:24" s="78" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A4" s="69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="70"/>
       <c r="C4" s="71"/>
       <c r="D4" s="72" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E4" s="73" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F4" s="72" t="s">
         <v>40</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H4" s="75"/>
       <c r="I4" s="72" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J4" s="69" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K4" s="76"/>
       <c r="L4" s="70"/>
@@ -4438,18 +4438,18 @@
       </c>
       <c r="R4" s="70"/>
       <c r="S4" s="69" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="T4" s="76"/>
       <c r="U4" s="69" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="V4" s="77"/>
       <c r="X4" s="71"/>
     </row>
     <row r="5" spans="1:24" s="83" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="79" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
@@ -4465,47 +4465,47 @@
     </row>
     <row r="6" spans="1:24" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="84" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" s="85"/>
       <c r="C6" s="86"/>
       <c r="D6" s="87" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="88" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="84" t="s">
-        <v>125</v>
-      </c>
       <c r="G6" s="88" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H6" s="86"/>
       <c r="I6" s="90" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J6" s="88" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K6" s="85"/>
       <c r="L6" s="85"/>
       <c r="M6" s="86"/>
       <c r="N6" s="88" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O6" s="85"/>
       <c r="P6" s="86"/>
       <c r="Q6" s="84" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="R6" s="85"/>
       <c r="S6" s="89" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="T6" s="85"/>
       <c r="U6" s="91" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="V6" s="86"/>
       <c r="X6" s="86"/>
@@ -4532,7 +4532,7 @@
     </row>
     <row r="8" spans="1:24" s="92" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="92" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" s="80"/>
       <c r="C8" s="80"/>
@@ -4575,7 +4575,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="60" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -4598,10 +4598,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -6215,7 +6215,7 @@
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -6301,12 +6301,12 @@
       <c r="Q1" s="121"/>
       <c r="R1" s="121"/>
       <c r="S1" s="106" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="T1" s="107"/>
       <c r="U1" s="108"/>
       <c r="V1" s="105" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W1" s="105"/>
     </row>
@@ -6353,13 +6353,13 @@
         <v>46</v>
       </c>
       <c r="T2" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U2" s="51" t="s">
         <v>48</v>
       </c>
       <c r="V2" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="W2" s="51" t="s">
         <v>48</v>
@@ -6367,7 +6367,7 @@
     </row>
     <row r="3" spans="1:26" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="52" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="53"/>
@@ -6480,7 +6480,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="N7" s="24" t="s">
         <v>23</v>
@@ -6495,22 +6495,22 @@
         <v>26</v>
       </c>
       <c r="R7" s="50" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S7" s="23" t="s">
         <v>4</v>
       </c>
       <c r="T7" s="22" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="U7" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="V7" s="99" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W7" s="100" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -6913,7 +6913,7 @@
   <dimension ref="A1:Y108"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6982,12 +6982,12 @@
       <c r="Q1" s="121"/>
       <c r="R1" s="121"/>
       <c r="S1" s="106" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="T1" s="107"/>
       <c r="U1" s="108"/>
       <c r="V1" s="105" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W1" s="105"/>
     </row>
@@ -7034,13 +7034,13 @@
         <v>46</v>
       </c>
       <c r="T2" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="U2" s="51" t="s">
         <v>48</v>
       </c>
       <c r="V2" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="W2" s="51" t="s">
         <v>48</v>
@@ -7048,7 +7048,7 @@
     </row>
     <row r="3" spans="1:25" s="18" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="52" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="53"/>
@@ -7159,7 +7159,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="N7" s="24" t="s">
         <v>23</v>
@@ -7174,22 +7174,22 @@
         <v>26</v>
       </c>
       <c r="R7" s="50" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S7" s="23" t="s">
         <v>4</v>
       </c>
       <c r="T7" s="22" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="U7" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="V7" s="99" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W7" s="100" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
@@ -7579,7 +7579,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="77" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="70" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -7595,7 +7595,7 @@
   <dimension ref="A1:W107"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T7" activeCellId="2" sqref="M7 R7 T7"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7824,7 +7824,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="N7" s="24" t="s">
         <v>23</v>
@@ -7839,13 +7839,13 @@
         <v>26</v>
       </c>
       <c r="R7" s="50" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S7" s="22" t="s">
         <v>4</v>
       </c>
       <c r="T7" s="49" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
@@ -8229,7 +8229,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="79" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="79" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -8245,7 +8245,7 @@
   <dimension ref="A1:W108"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:T7"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8471,7 +8471,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="N7" s="24" t="s">
         <v>23</v>
@@ -8486,13 +8486,13 @@
         <v>26</v>
       </c>
       <c r="R7" s="50" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S7" s="22" t="s">
         <v>4</v>
       </c>
       <c r="T7" s="49" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
@@ -8877,7 +8877,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="79" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="75" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -8893,7 +8893,7 @@
   <dimension ref="A1:V102"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:S1"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8958,7 +8958,7 @@
         <v>46</v>
       </c>
       <c r="R1" s="105" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="S1" s="105"/>
       <c r="U1"/>
@@ -8983,7 +8983,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M2" s="16">
         <v>1</v>
@@ -8995,11 +8995,11 @@
         <v>3</v>
       </c>
       <c r="P2" s="96" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q2" s="133"/>
       <c r="R2" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S2" s="51" t="s">
         <v>48</v>
@@ -9007,7 +9007,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -9039,7 +9039,7 @@
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F4" s="27" t="s">
         <v>2</v>
@@ -9078,13 +9078,13 @@
         <v>4</v>
       </c>
       <c r="R4" s="99" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S4" s="100" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="V4" s="101" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -9430,7 +9430,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="74" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="75" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -9446,7 +9446,7 @@
   <dimension ref="A1:S97"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:S1"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9509,7 +9509,7 @@
         <v>46</v>
       </c>
       <c r="R1" s="105" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="S1" s="105"/>
     </row>
@@ -9532,7 +9532,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M2" s="16">
         <v>1</v>
@@ -9544,11 +9544,11 @@
         <v>3</v>
       </c>
       <c r="P2" s="96" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q2" s="133"/>
       <c r="R2" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S2" s="51" t="s">
         <v>48</v>
@@ -9556,7 +9556,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -9585,7 +9585,7 @@
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F4" s="27" t="s">
         <v>2</v>
@@ -9624,10 +9624,10 @@
         <v>4</v>
       </c>
       <c r="R4" s="99" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="S4" s="100" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -9954,7 +9954,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="73" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -9970,7 +9970,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:P1048576"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9989,7 +9989,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10015,13 +10015,13 @@
         <v>42</v>
       </c>
       <c r="N3" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="O3" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="P3" s="64" t="s">
         <v>146</v>
-      </c>
-      <c r="O3" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="P3" s="64" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -10054,13 +10054,13 @@
         <v>9</v>
       </c>
       <c r="N5" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="P5" s="102" t="s">
         <v>149</v>
-      </c>
-      <c r="O5" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="P5" s="102" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -10112,13 +10112,13 @@
         <v>46</v>
       </c>
       <c r="H10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>50</v>
@@ -10130,13 +10130,13 @@
         <v>51</v>
       </c>
       <c r="N10" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="O10" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="P10" s="64" t="s">
         <v>146</v>
-      </c>
-      <c r="O10" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="P10" s="64" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -10174,31 +10174,31 @@
         <v>4</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>39</v>
       </c>
       <c r="L12" s="62" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M12" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N12" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="O12" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="N12" s="62" t="s">
+      <c r="P12" s="62" t="s">
         <v>153</v>
-      </c>
-      <c r="O12" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="P12" s="62" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -10270,7 +10270,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="71" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -10289,7 +10289,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:P1048576"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10307,7 +10307,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10341,13 +10341,13 @@
         <v>42</v>
       </c>
       <c r="N3" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="O3" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="P3" s="64" t="s">
         <v>146</v>
-      </c>
-      <c r="O3" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="P3" s="64" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -10386,13 +10386,13 @@
         <v>9</v>
       </c>
       <c r="N5" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="P5" s="102" t="s">
         <v>149</v>
-      </c>
-      <c r="O5" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="P5" s="102" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -10459,13 +10459,13 @@
         <v>46</v>
       </c>
       <c r="H10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>50</v>
@@ -10477,18 +10477,18 @@
         <v>51</v>
       </c>
       <c r="N10" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="O10" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="P10" s="64" t="s">
         <v>146</v>
-      </c>
-      <c r="O10" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="P10" s="64" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -10523,31 +10523,31 @@
         <v>4</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>39</v>
       </c>
       <c r="L12" s="62" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M12" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="N12" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="O12" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="N12" s="62" t="s">
+      <c r="P12" s="62" t="s">
         <v>153</v>
-      </c>
-      <c r="O12" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="P12" s="62" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -10661,7 +10661,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.43307086614173229" header="0.23622047244094491" footer="0.15748031496062992"/>
-  <pageSetup scale="74" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="67" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;14Classement Sinclair - Sinclair Ranking&amp;R&amp;14Hommes - Men</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>

</xml_diff>